<commit_message>
dummy file for sc
</commit_message>
<xml_diff>
--- a/SC.xlsx
+++ b/SC.xlsx
@@ -21,6 +21,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,10 +377,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>